<commit_message>
feat: perform inferSent query
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F24AA51-8809-EA4D-8165-1145A2809133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7288B17-D8FD-BC40-9AC8-5E882B2CA961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="1520" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="-36480" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Task</t>
   </si>
@@ -140,9 +140,6 @@
     <t xml:space="preserve">PROBLEM: Elasticsearch max. dimension of dense vector is 2048, vocab size of corpus is bigger (7243), SOLUTION: create multple features/ properties for large vector and search multiple times when querying OR use PCA/ AE to reduce dimensionality </t>
   </si>
   <si>
-    <t>InferSent: + encoder layer of AE to reduce dimensionality</t>
-  </si>
-  <si>
     <t>Cluster: bewerten lassen</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>BA: Pipeline Bild s. Christians Zeichnung, 62GB Daten -&gt; offline verarbeiten -&gt; DB -&gt; auf kleinem System durchsuchbar</t>
   </si>
   <si>
-    <t>try Convolutional AE</t>
-  </si>
-  <si>
     <t>try AE with higher dimensionality and use PCA to visualize</t>
   </si>
   <si>
@@ -203,7 +197,16 @@
     <t>why are cluster sizes of PCA results imbalanced? Because they are too sparse</t>
   </si>
   <si>
-    <t>TFIDF: strip accents in db embedding, created preprocessing class which can be used instead of default preprocessor, added TFIDF all-zero-flag, restructured repo: run everything from main.py now</t>
+    <t>TFIDF: strip accents in db embedding, created preprocessing class which can be used instead of default preprocessor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> added TFIDF all-zero-flag, restructured repo: run everything from main.py now</t>
+  </si>
+  <si>
+    <t>try Convolutional AE: https://blog.keras.io/building-autoencoders-in-keras.html</t>
+  </si>
+  <si>
+    <t>InferSent: + encoder layer of AE to reduce dimensionality in db &amp; query (bad results) possible</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -421,6 +424,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -428,9 +437,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -754,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -779,7 +785,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="18">
+      <c r="A2" s="20">
         <v>45144</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -790,7 +796,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
@@ -799,7 +805,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
@@ -808,7 +814,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
@@ -896,7 +902,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -938,9 +944,6 @@
       <c r="B18" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="19" spans="1:4" ht="154" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
@@ -950,7 +953,7 @@
         <v>29</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -961,7 +964,7 @@
         <v>30</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -972,7 +975,7 @@
         <v>31</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -983,88 +986,100 @@
         <v>32</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
         <v>45168</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D23" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="19">
+        <v>45169</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="D24" s="8" t="s">
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="19">
+        <v>45170</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D25" s="8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D26" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D27" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D28" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D29" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D30" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D31" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D32" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" ht="17" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D33" s="8" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D34" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="4:4" ht="51" x14ac:dyDescent="0.2">
       <c r="D35" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D36" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D37" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added interactive cluster algo comparison
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7288B17-D8FD-BC40-9AC8-5E882B2CA961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7406EDD-2B82-4F4C-80F0-B32493BCDF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36480" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Task</t>
   </si>
@@ -122,9 +122,6 @@
     <t>multiple tfidf vectors for different tasks (1. similarity between documents omitting words which occur only once in the corpus, 2. finding specific documents omitting words which occur in every document, etc.) -&gt; reduce vector size (=#unique words), BA: assumption is that there are similarities (content wise and in terms of visual appearance) between documents of same type (eg. Urkunde)</t>
   </si>
   <si>
-    <t>Google's universal Sentence Encoder: Alter shapes to fix problem (HOW?)</t>
-  </si>
-  <si>
     <t>InferSent hypothese: project does not support training: https://github.com/facebookresearch/InferSent/issues/82 , Universal Sentence Encoder: the embedding uses n-grams of documents close to current doc (like a window) to embed it, cf. DAN in https://amitness.com/2020/06/universal-sentence-encoder/ -&gt; unable to fix subtraction problem, started working on eigenfaces</t>
   </si>
   <si>
@@ -143,12 +140,6 @@
     <t>Cluster: bewerten lassen</t>
   </si>
   <si>
-    <t>Cluster Algo: DBSCAN (nicht parametrisch != Kmeans)</t>
-  </si>
-  <si>
-    <t>Cluster Algo: HDBSCAN  (nicht parametrisch != Kmeans)</t>
-  </si>
-  <si>
     <t>Cluster Algo: OPTICS (nicht parametrisch != Kmeans)</t>
   </si>
   <si>
@@ -206,7 +197,10 @@
     <t>try Convolutional AE: https://blog.keras.io/building-autoencoders-in-keras.html</t>
   </si>
   <si>
-    <t>InferSent: + encoder layer of AE to reduce dimensionality in db &amp; query (bad results) possible</t>
+    <t>Google's universal Sentence Encoder: Alter shapes to fix problem (HOW?), InferSent has same difference problem</t>
+  </si>
+  <si>
+    <t>InferSent: + encoder layer of AE to reduce dimensionality in db &amp; query (bad results) possible, compared (interactively) Cluster Algos: DBSCAN (nicht parametrisch != Kmeans), HDBSCAN  (nicht parametrisch != Kmeans), KMeans</t>
   </si>
 </sst>
 </file>
@@ -371,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -425,9 +419,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -760,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -785,7 +776,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="20">
+      <c r="A2" s="19">
         <v>45144</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -796,7 +787,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="21"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
@@ -805,7 +796,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
@@ -814,7 +805,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
@@ -830,7 +821,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -861,7 +852,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -902,7 +893,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -950,10 +941,7 @@
         <v>45163</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -961,10 +949,7 @@
         <v>45164</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -972,10 +957,10 @@
         <v>45167</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -983,10 +968,10 @@
         <v>45168</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
@@ -994,92 +979,92 @@
         <v>45168</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="19">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
         <v>45169</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>45170</v>
+      </c>
+      <c r="B25" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="19">
-        <v>45170</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="D25" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D26" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D27" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D28" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D29" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D30" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D31" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D32" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D33" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D34" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="4:4" ht="51" x14ac:dyDescent="0.2">
       <c r="D35" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D36" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D37" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added clustering algo OPTICS comparison
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7406EDD-2B82-4F4C-80F0-B32493BCDF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396E064D-ADE1-F14F-89A7-10BD03F20F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36480" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Task</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Cluster: bewerten lassen</t>
   </si>
   <si>
-    <t>Cluster Algo: OPTICS (nicht parametrisch != Kmeans)</t>
-  </si>
-  <si>
     <t>Cluster für Bilder und Text nutzbar</t>
   </si>
   <si>
@@ -200,7 +197,7 @@
     <t>Google's universal Sentence Encoder: Alter shapes to fix problem (HOW?), InferSent has same difference problem</t>
   </si>
   <si>
-    <t>InferSent: + encoder layer of AE to reduce dimensionality in db &amp; query (bad results) possible, compared (interactively) Cluster Algos: DBSCAN (nicht parametrisch != Kmeans), HDBSCAN  (nicht parametrisch != Kmeans), KMeans</t>
+    <t>InferSent: + encoder layer of AE to reduce dimensionality in db &amp; query (bad results) possible, compared (interactively) Cluster Algos: DBSCAN (nicht parametrisch != Kmeans), HDBSCAN  (nicht parametrisch != Kmeans),  OPTICS (nicht parametrisch != Kmeans), KMeans</t>
   </si>
 </sst>
 </file>
@@ -752,7 +749,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,7 +849,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -893,7 +890,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -959,9 +956,6 @@
       <c r="B21" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
@@ -979,10 +973,10 @@
         <v>45168</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -990,81 +984,81 @@
         <v>45169</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="103" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>45170</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D26" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D27" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D28" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D29" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D30" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D31" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D32" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D33" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D34" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="4:4" ht="51" x14ac:dyDescent="0.2">
       <c r="D35" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D36" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D37" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: saved different clusterings to json
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396E064D-ADE1-F14F-89A7-10BD03F20F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7495A0B3-1AA5-6949-AC29-800D05B76412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36480" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -362,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -425,6 +425,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -748,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1002,6 +1005,9 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="22">
+        <v>45171</v>
+      </c>
       <c r="D26" s="8" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
feat: added first 4 components visualization
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7495A0B3-1AA5-6949-AC29-800D05B76412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6EA255-7DBE-974A-A8E0-7FFB496CD12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -362,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -425,9 +425,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -751,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1004,9 +1001,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="22">
+    <row r="26" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
         <v>45171</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>37</v>
@@ -1015,11 +1015,6 @@
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D27" s="8" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="D28" s="8" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: added BayesianGaussianMixture cluster comp
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6EA255-7DBE-974A-A8E0-7FFB496CD12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD3660A-83C3-8547-BD1D-2680699EFE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Task</t>
   </si>
@@ -155,15 +155,6 @@
     <t>Eigenfaces: hohe dim &lt;-&gt; sparse &lt;-&gt; Clustern schwer</t>
   </si>
   <si>
-    <t>Eigenfaces: 3-4 components, visualize via 3d scatter plot (matplotlib)/ 4d via colors</t>
-  </si>
-  <si>
-    <t>Cluster Algo: Variationale Baysian Mixture Model after PCA</t>
-  </si>
-  <si>
-    <t>Eigenfaces: display Entwicklung von Rekonstruktionsfehler, way to find best # components</t>
-  </si>
-  <si>
     <t>BA: Pipeline Bild s. Christians Zeichnung, 62GB Daten -&gt; offline verarbeiten -&gt; DB -&gt; auf kleinem System durchsuchbar</t>
   </si>
   <si>
@@ -198,6 +189,9 @@
   </si>
   <si>
     <t>InferSent: + encoder layer of AE to reduce dimensionality in db &amp; query (bad results) possible, compared (interactively) Cluster Algos: DBSCAN (nicht parametrisch != Kmeans), HDBSCAN  (nicht parametrisch != Kmeans),  OPTICS (nicht parametrisch != Kmeans), KMeans</t>
+  </si>
+  <si>
+    <t>Eigenfaces: 3-4 components, visualize via 3d scatter plot (matplotlib)/ 4d via colors, Eigenfaces: display Entwicklung von Rekonstruktionsfehler: way to find best # components, added Cluster Algo: Variationale Baysian Mixture Model after PCA</t>
   </si>
 </sst>
 </file>
@@ -749,7 +743,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -849,7 +843,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -890,7 +884,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -973,7 +967,7 @@
         <v>45168</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>34</v>
@@ -984,7 +978,7 @@
         <v>45169</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>35</v>
@@ -995,18 +989,18 @@
         <v>45170</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>45171</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>37</v>
@@ -1017,49 +1011,39 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="D29" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D30" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D31" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D32" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D33" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D34" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="4:4" ht="51" x14ac:dyDescent="0.2">
       <c r="D35" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D36" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D37" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: usage of euclidean distance for residuals
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD3660A-83C3-8547-BD1D-2680699EFE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B2C6B6-0FE4-894F-9820-725302E0C887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Task</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Eigenfaces: 3-4 components, visualize via 3d scatter plot (matplotlib)/ 4d via colors, Eigenfaces: display Entwicklung von Rekonstruktionsfehler: way to find best # components, added Cluster Algo: Variationale Baysian Mixture Model after PCA</t>
+  </si>
+  <si>
+    <t>Why are residual graph so similar for both latent dimensions?</t>
   </si>
 </sst>
 </file>
@@ -743,7 +746,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1011,6 +1014,11 @@
         <v>38</v>
       </c>
     </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D29" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D31" s="8" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
feat: compared higher dim AE on 2d PCA
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B2C6B6-0FE4-894F-9820-725302E0C887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2774BE96-F2A9-0945-BAEF-0653B7365E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Task</t>
   </si>
@@ -158,9 +158,6 @@
     <t>BA: Pipeline Bild s. Christians Zeichnung, 62GB Daten -&gt; offline verarbeiten -&gt; DB -&gt; auf kleinem System durchsuchbar</t>
   </si>
   <si>
-    <t>try AE with higher dimensionality and use PCA to visualize</t>
-  </si>
-  <si>
     <t xml:space="preserve">BA: AE latent space normal verteilt???? </t>
   </si>
   <si>
@@ -191,10 +188,10 @@
     <t>InferSent: + encoder layer of AE to reduce dimensionality in db &amp; query (bad results) possible, compared (interactively) Cluster Algos: DBSCAN (nicht parametrisch != Kmeans), HDBSCAN  (nicht parametrisch != Kmeans),  OPTICS (nicht parametrisch != Kmeans), KMeans</t>
   </si>
   <si>
-    <t>Eigenfaces: 3-4 components, visualize via 3d scatter plot (matplotlib)/ 4d via colors, Eigenfaces: display Entwicklung von Rekonstruktionsfehler: way to find best # components, added Cluster Algo: Variationale Baysian Mixture Model after PCA</t>
-  </si>
-  <si>
     <t>Why are residual graph so similar for both latent dimensions?</t>
+  </si>
+  <si>
+    <t>Eigenfaces: 3-4 components, visualize via 3d scatter plot (matplotlib)/ 4d via colors, Eigenfaces: display Entwicklung von Rekonstruktionsfehler: way to find best # components, added Cluster Algo: Variationale Baysian Mixture Model after PCA, try AE with higher dimensionality and use PCA to visualize</t>
   </si>
 </sst>
 </file>
@@ -746,7 +743,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -846,7 +843,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -887,7 +884,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -970,7 +967,7 @@
         <v>45168</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>34</v>
@@ -981,7 +978,7 @@
         <v>45169</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>35</v>
@@ -992,13 +989,13 @@
         <v>45170</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="103" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>45171</v>
       </c>
@@ -1016,7 +1013,7 @@
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D29" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1026,32 +1023,27 @@
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D32" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D33" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D34" s="8" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="4:4" ht="51" x14ac:dyDescent="0.2">
       <c r="D35" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D36" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D37" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added convolutional AE
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2774BE96-F2A9-0945-BAEF-0653B7365E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F923EFB-580C-DE4B-B173-AE3FF979B051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -179,9 +179,6 @@
     <t xml:space="preserve"> added TFIDF all-zero-flag, restructured repo: run everything from main.py now</t>
   </si>
   <si>
-    <t>try Convolutional AE: https://blog.keras.io/building-autoencoders-in-keras.html</t>
-  </si>
-  <si>
     <t>Google's universal Sentence Encoder: Alter shapes to fix problem (HOW?), InferSent has same difference problem</t>
   </si>
   <si>
@@ -191,7 +188,10 @@
     <t>Why are residual graph so similar for both latent dimensions?</t>
   </si>
   <si>
-    <t>Eigenfaces: 3-4 components, visualize via 3d scatter plot (matplotlib)/ 4d via colors, Eigenfaces: display Entwicklung von Rekonstruktionsfehler: way to find best # components, added Cluster Algo: Variationale Baysian Mixture Model after PCA, try AE with higher dimensionality and use PCA to visualize</t>
+    <t xml:space="preserve">Eigenfaces: 3-4 components, visualize via 3d scatter plot (matplotlib)/ 4d via colors, Eigenfaces: display Entwicklung von Rekonstruktionsfehler: way to find best # components, added Cluster Algo: Variationale Baysian Mixture Model after PCA, try AE with higher dimensionality and use PCA to visualize, tried Convolutional AE: https://blog.keras.io/building-autoencoders-in-keras.html </t>
+  </si>
+  <si>
+    <t>Conv. AE is bad</t>
   </si>
 </sst>
 </file>
@@ -356,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -420,6 +420,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -740,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -831,7 +834,7 @@
       <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -843,7 +846,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -853,6 +856,9 @@
       <c r="B10" s="14" t="s">
         <v>20</v>
       </c>
+      <c r="D10" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
@@ -862,7 +868,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -873,7 +879,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
@@ -884,7 +890,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -894,6 +900,9 @@
       <c r="B14" s="14" t="s">
         <v>18</v>
       </c>
+      <c r="D14" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
@@ -902,6 +911,9 @@
       <c r="B15" s="10" t="s">
         <v>19</v>
       </c>
+      <c r="D15" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
@@ -910,6 +922,9 @@
       <c r="B16" s="17" t="s">
         <v>22</v>
       </c>
+      <c r="D16" s="22" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
@@ -918,6 +933,9 @@
       <c r="B17" s="14" t="s">
         <v>26</v>
       </c>
+      <c r="D17" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="137" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
@@ -926,6 +944,9 @@
       <c r="B18" s="14" t="s">
         <v>27</v>
       </c>
+      <c r="D18" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="154" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
@@ -942,6 +963,9 @@
       <c r="B20" s="14" t="s">
         <v>29</v>
       </c>
+      <c r="D20" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
@@ -951,7 +975,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>45168</v>
       </c>
@@ -959,7 +983,7 @@
         <v>31</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
@@ -970,7 +994,7 @@
         <v>45</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -980,70 +1004,39 @@
       <c r="B24" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="25" spans="1:4" ht="103" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>45170</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="137" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>45171</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D27" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D28" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D29" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="D31" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D32" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="D33" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="D35" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D36" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D37" s="8" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: changed method name
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CE38D8-CF5C-F445-A384-09C87D6489BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B7B3C8-02BB-6647-8AB4-F83A5824DE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>Task</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>added Wordcloud for one document to UI V2, VSCode on cluster</t>
+  </si>
+  <si>
+    <t>fuzzy full-text search</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -494,9 +497,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1181,29 +1181,35 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="25">
+    <row r="35" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
         <v>45182</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="14" t="s">
         <v>73</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="25">
+    <row r="36" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
         <v>45183</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="14" t="s">
         <v>72</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <v>45184</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>74</v>
+      </c>
       <c r="D37" s="8" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
feat: OPTICS & eigendocs vs. 32x32
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1409693-55A8-4147-B6F7-B613F9FFA729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0093E4F2-81D9-B04E-A127-8DBCDA1B5B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -257,28 +257,28 @@
     <t>added Wordcloud for one document to UI V2, VSCode on cluster</t>
   </si>
   <si>
-    <t>fuzzy full-text search</t>
-  </si>
-  <si>
     <t xml:space="preserve">reduce tfidf vocab </t>
   </si>
   <si>
-    <t>eigendocs code</t>
-  </si>
-  <si>
-    <t>eigendocs BA</t>
-  </si>
-  <si>
-    <t>OPTICS: threshold hierarchical clustering, reduce threshold and observe new documents</t>
-  </si>
-  <si>
     <t>database on cluster</t>
   </si>
   <si>
     <t>id are hashes of text</t>
   </si>
   <si>
-    <t>PCA: 32 dim, cluster with OPTICS</t>
+    <t>BA: Clustering</t>
+  </si>
+  <si>
+    <t>fuzzy full-text search, DB: Elasticsearch</t>
+  </si>
+  <si>
+    <t>OPTICS: reachability plot + clustering</t>
+  </si>
+  <si>
+    <t>OPTICS: on 32x32 and on PCA version (PCA/eigendoc is better), PCA on 2^2, 5^2, 14^2 -&gt; 2^2 is best, eigendocs code und BA</t>
+  </si>
+  <si>
+    <t>OPTICS: threshold hierarchical clustering, reduce threshold and observe new documents -&gt; schwer</t>
   </si>
 </sst>
 </file>
@@ -836,7 +836,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1223,7 +1223,7 @@
         <v>45184</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>60</v>
@@ -1234,55 +1234,58 @@
         <v>45185</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13">
+        <v>45186</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>76</v>
+      </c>
       <c r="D39" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
+        <v>45187</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="D40" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
+        <v>45188</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="D41" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D42" s="19" t="s">
-        <v>80</v>
-      </c>
-    </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D43" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D44" s="19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D45" s="19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D46" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D47" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: only save new documents
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEC87B1-8E55-1447-9A21-62BCD7000F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F71FF4-C503-2549-8903-232B2DF19B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -242,9 +242,6 @@
     <t>added Wordcloud for one document to UI V2, VSCode on cluster</t>
   </si>
   <si>
-    <t xml:space="preserve">reduce tfidf vocab </t>
-  </si>
-  <si>
     <t>database on cluster</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>OPTICS: on 32x32 and on PCA version (PCA/eigendoc is better), PCA on 2^2, 5^2, 14^2 -&gt; 2^2 is best, eigendocs code und BA: eigendocs</t>
+  </si>
+  <si>
+    <t>reduce tfidf vocab : SVD/ https://stackoverflow.com/questions/61274499/reduce-dimension-of-word-vectors-from-tfidfvectorizer-countvectorizer</t>
   </si>
 </sst>
 </file>
@@ -824,7 +824,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1196,7 +1196,7 @@
         <v>45184</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>55</v>
@@ -1207,7 +1207,7 @@
         <v>45185</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>57</v>
@@ -1218,7 +1218,7 @@
         <v>45186</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>58</v>
@@ -1229,7 +1229,7 @@
         <v>45187</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>59</v>
@@ -1240,25 +1240,25 @@
         <v>45188</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="D43" s="8" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D45" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D47" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
style: code clean up
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70662C4-FD6D-C049-89F1-39A929B02C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9564788E-15F6-6547-80B6-D3E0999057A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-140" yWindow="820" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="0" yWindow="820" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -284,9 +284,6 @@
     <t>BA: pro section: first problem, then how to solve it, then techniques used</t>
   </si>
   <si>
-    <t>Init_db: multiprocessng</t>
-  </si>
-  <si>
     <t># PCA components from cumulative explained variance knee/ or reconstrcution error (4-20 total)</t>
   </si>
   <si>
@@ -297,6 +294,9 @@
   </si>
   <si>
     <t>BA: SVD gibt Bausteine, mittelwert automatisch in Implementierung, aber wichtig in Text</t>
+  </si>
+  <si>
+    <t>Init_db: multiprocessing</t>
   </si>
 </sst>
 </file>
@@ -857,7 +857,7 @@
   <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="52" spans="4:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D52" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="4:4" ht="17" x14ac:dyDescent="0.2">
@@ -1336,22 +1336,22 @@
     </row>
     <row r="55" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D55" s="8" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D56" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="4:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D57" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="4:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D58" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: improved visual of UI
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FC716B-9FE0-3049-A3A5-0E709747F747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DEF599-0119-B74B-8922-C2CFA3D341EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>Task</t>
   </si>
@@ -278,9 +278,6 @@
     <t>BA: pro section: first problem, then how to solve it, then techniques used</t>
   </si>
   <si>
-    <t>cluster: argmax(pca weights)</t>
-  </si>
-  <si>
     <t>BA: related work section 3, 2=fundamentals/state of the art, etc. cf. 20.09.2023 Vortrag</t>
   </si>
   <si>
@@ -291,6 +288,12 @@
   </si>
   <si>
     <t>hash: of bytes of file, # PCA components from cumulative explained variance knee/ or reconstrcution error (4-20 total), 32x32 -&gt; PCA -&gt; OPTICS, Init_db: multiprocessing</t>
+  </si>
+  <si>
+    <t>cluster: argmax(pca weights), clustering on 13 instead of 2dims</t>
+  </si>
+  <si>
+    <t>change clusters in db to eigendocs + OPTICS</t>
   </si>
 </sst>
 </file>
@@ -455,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -524,12 +527,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -853,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1143,7 +1140,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="25">
+      <c r="A29" s="13">
         <v>45174</v>
       </c>
       <c r="B29" s="14" t="s">
@@ -1203,7 +1200,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="25">
+      <c r="A35" s="13">
         <v>45182</v>
       </c>
       <c r="B35" s="14" t="s">
@@ -1281,7 +1278,7 @@
         <v>45189</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
@@ -1289,18 +1286,21 @@
         <v>45190</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="24">
+    <row r="44" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="13">
         <v>45191</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>80</v>
+      <c r="B44" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1335,12 +1335,12 @@
     </row>
     <row r="57" spans="4:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D57" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="4:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D58" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: inserting only certain embeddings in db
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DEF599-0119-B74B-8922-C2CFA3D341EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF1187F-13B9-704F-A008-25EF6ABCAD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="1920" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
   <si>
     <t>Task</t>
   </si>
@@ -278,22 +278,22 @@
     <t>BA: pro section: first problem, then how to solve it, then techniques used</t>
   </si>
   <si>
-    <t>BA: related work section 3, 2=fundamentals/state of the art, etc. cf. 20.09.2023 Vortrag</t>
-  </si>
-  <si>
-    <t>BA: SVD gibt Bausteine, mittelwert automatisch in Implementierung, aber wichtig in Text</t>
-  </si>
-  <si>
     <t>work event</t>
   </si>
   <si>
     <t>hash: of bytes of file, # PCA components from cumulative explained variance knee/ or reconstrcution error (4-20 total), 32x32 -&gt; PCA -&gt; OPTICS, Init_db: multiprocessing</t>
   </si>
   <si>
-    <t>cluster: argmax(pca weights), clustering on 13 instead of 2dims</t>
-  </si>
-  <si>
     <t>change clusters in db to eigendocs + OPTICS</t>
+  </si>
+  <si>
+    <t>cluster: argmax(pca weights), clustering on 13 instead of 2dims, BA: related work section 3, 2=fundamentals/state of the art, etc. cf. 20.09.2023 Vortrag, BA: SVD gibt Bausteine, mittelwert automatisch in Implementierung, aber wichtig in Text</t>
+  </si>
+  <si>
+    <t>termfrequency</t>
+  </si>
+  <si>
+    <t>BA: soft cosine similarity</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -518,6 +518,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -848,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,7 +878,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="21">
+      <c r="A2" s="22">
         <v>45144</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -886,7 +889,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="22"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
@@ -895,7 +898,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
@@ -904,7 +907,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>45189</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
@@ -1286,29 +1289,49 @@
         <v>45190</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="103" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>45191</v>
       </c>
       <c r="B44" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="13">
+        <v>45192</v>
+      </c>
+      <c r="B45" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D45" s="19" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="21">
+        <v>45193</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="13">
+        <v>45194</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="D47" s="8" t="s">
         <v>68</v>
       </c>
@@ -1331,16 +1354,6 @@
     <row r="54" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D54" s="8" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="D57" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="58" spans="4:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="D58" s="8" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: try only one embedding
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF1187F-13B9-704F-A008-25EF6ABCAD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A31F03-3920-174E-AA50-450887DE9543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>Task</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>BA: soft cosine similarity</t>
+  </si>
+  <si>
+    <t>insert only certain embeddings into db, BA: term frequency, (soft) cosine sim.</t>
   </si>
 </sst>
 </file>
@@ -854,7 +857,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1336,6 +1339,14 @@
         <v>68</v>
       </c>
     </row>
+    <row r="48" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="13">
+        <v>45195</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
     <row r="49" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D49" s="8" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
feat: find times per embedding execution
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A31F03-3920-174E-AA50-450887DE9543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097B2C0B-9593-5C4B-A374-841ED0444DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="1920" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
   <si>
     <t>Task</t>
   </si>
@@ -257,9 +257,6 @@
     <t>OPTICS: threshold hierarchical clustering, reduce threshold and observe new documents -&gt; schwer</t>
   </si>
   <si>
-    <t>reduce tfidf vocab : SVD/ https://stackoverflow.com/questions/61274499/reduce-dimension-of-word-vectors-from-tfidfvectorizer-countvectorizer</t>
-  </si>
-  <si>
     <t>id are hashes of text, only add new docs</t>
   </si>
   <si>
@@ -297,6 +294,30 @@
   </si>
   <si>
     <t>insert only certain embeddings into db, BA: term frequency, (soft) cosine sim.</t>
+  </si>
+  <si>
+    <t>AE: 0% reconstruction error</t>
+  </si>
+  <si>
+    <t>RSME usage for PCA reconstruction error</t>
+  </si>
+  <si>
+    <t>BA: high level eval of image clustering etc.</t>
+  </si>
+  <si>
+    <t>BA: qualitativ für 195 docs  eval (Vorstellung vs Realität, welche Merkmale fallen auf?)</t>
+  </si>
+  <si>
+    <t>besten Algo auf labeled doc clustering Datensatz finden</t>
+  </si>
+  <si>
+    <t>Eval: Metrik für Cluster finden</t>
+  </si>
+  <si>
+    <t>Eval: semantic vs layout basiert Verfahren (vgl)</t>
+  </si>
+  <si>
+    <t>reduce tfidf vocab : SVD/ https://stackoverflow.com/questions/61274499/reduce-dimension-of-word-vectors-from-tfidfvectorizer-countvectorizer , https://scikit-learn.org/stable/auto_examples/text/plot_document_clustering.html LSA !!!!</t>
   </si>
 </sst>
 </file>
@@ -854,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1240,7 +1261,7 @@
         <v>45185</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>57</v>
@@ -1273,7 +1294,7 @@
         <v>45188</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>60</v>
@@ -1284,18 +1305,18 @@
         <v>45189</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>45190</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="103" thickBot="1" x14ac:dyDescent="0.25">
@@ -1303,10 +1324,10 @@
         <v>45191</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -1314,7 +1335,7 @@
         <v>45192</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D45" s="19" t="s">
         <v>72</v>
@@ -1325,7 +1346,7 @@
         <v>45193</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1344,27 +1365,63 @@
         <v>45195</v>
       </c>
       <c r="B48" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13">
+        <v>45196</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D50" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D51" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D54" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D55" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="4:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D49" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D50" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="4:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D51" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D54" s="8" t="s">
-        <v>79</v>
+    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D56" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="D57" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D58" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D59" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D60" s="8" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: updated field name in database
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097B2C0B-9593-5C4B-A374-841ED0444DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE87B0DD-4C77-1049-96D7-FF9000A73442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -299,9 +299,6 @@
     <t>AE: 0% reconstruction error</t>
   </si>
   <si>
-    <t>RSME usage for PCA reconstruction error</t>
-  </si>
-  <si>
     <t>BA: high level eval of image clustering etc.</t>
   </si>
   <si>
@@ -318,6 +315,9 @@
   </si>
   <si>
     <t>reduce tfidf vocab : SVD/ https://stackoverflow.com/questions/61274499/reduce-dimension-of-word-vectors-from-tfidfvectorizer-countvectorizer , https://scikit-learn.org/stable/auto_examples/text/plot_document_clustering.html LSA !!!!</t>
+  </si>
+  <si>
+    <t>RSME usage for PCA reconstruction error, time per embedding, fix AE dimension, argmax cluster on white canvas input, BA: tokenization etc.</t>
   </si>
 </sst>
 </file>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1316,7 +1316,7 @@
         <v>79</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="103" thickBot="1" x14ac:dyDescent="0.25">
@@ -1368,12 +1368,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>45196</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>75</v>
@@ -1401,27 +1401,27 @@
     </row>
     <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D56" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D57" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D58" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D59" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D60" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: code clean up
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE87B0DD-4C77-1049-96D7-FF9000A73442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC17BC01-989F-EA4B-8B91-EF80F91D22B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -281,9 +281,6 @@
     <t>hash: of bytes of file, # PCA components from cumulative explained variance knee/ or reconstrcution error (4-20 total), 32x32 -&gt; PCA -&gt; OPTICS, Init_db: multiprocessing</t>
   </si>
   <si>
-    <t>change clusters in db to eigendocs + OPTICS</t>
-  </si>
-  <si>
     <t>cluster: argmax(pca weights), clustering on 13 instead of 2dims, BA: related work section 3, 2=fundamentals/state of the art, etc. cf. 20.09.2023 Vortrag, BA: SVD gibt Bausteine, mittelwert automatisch in Implementierung, aber wichtig in Text</t>
   </si>
   <si>
@@ -318,6 +315,9 @@
   </si>
   <si>
     <t>RSME usage for PCA reconstruction error, time per embedding, fix AE dimension, argmax cluster on white canvas input, BA: tokenization etc.</t>
+  </si>
+  <si>
+    <t>BA: TFIDF, Doc2Vec</t>
   </si>
 </sst>
 </file>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1316,7 +1316,7 @@
         <v>79</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="103" thickBot="1" x14ac:dyDescent="0.25">
@@ -1324,9 +1324,6 @@
         <v>45191</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="D44" s="8" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1335,7 +1332,7 @@
         <v>45192</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D45" s="19" t="s">
         <v>72</v>
@@ -1346,7 +1343,7 @@
         <v>45193</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1365,7 +1362,7 @@
         <v>45195</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
@@ -1373,18 +1370,28 @@
         <v>45196</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="13">
+        <v>45197</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>93</v>
+      </c>
       <c r="D50" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="13">
+        <v>45198</v>
+      </c>
+      <c r="B51" s="14"/>
       <c r="D51" s="8" t="s">
         <v>77</v>
       </c>
@@ -1396,32 +1403,32 @@
     </row>
     <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D55" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D56" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D57" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D58" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D59" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D60" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: use default doc2vec model
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7216234-774C-4D49-99D5-47705C892279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE035E6-6942-934C-B590-5E81B8945AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
   <si>
     <t>Task</t>
   </si>
@@ -330,6 +330,12 @@
   </si>
   <si>
     <t>infersent: provide smaller word2vec vocab?</t>
+  </si>
+  <si>
+    <t>new times for embeddings</t>
+  </si>
+  <si>
+    <t>BA: doc2vec impl, doc2vec default model</t>
   </si>
 </sst>
 </file>
@@ -889,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1413,6 +1419,22 @@
         <v>77</v>
       </c>
     </row>
+    <row r="52" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="13">
+        <v>45199</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13">
+        <v>45200</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
     <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D54" s="8" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
feat: custom word2vec for inferSent
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE035E6-6942-934C-B590-5E81B8945AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EE29B5-59FE-E24D-870A-395ACE2AB2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
   <si>
     <t>Task</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>BA: doc2vec impl, doc2vec default model</t>
+  </si>
+  <si>
+    <t>BA: infersent, custom w2v for infersent</t>
   </si>
 </sst>
 </file>
@@ -896,7 +899,7 @@
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1435,7 +1438,13 @@
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="13">
+        <v>45201</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>100</v>
+      </c>
       <c r="D54" s="8" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
fix: 3d  cluster for white canvas images
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EE29B5-59FE-E24D-870A-395ACE2AB2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB0AA9D-8240-0D4F-94BC-FCF6962F9343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="38400" yWindow="560" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -326,12 +326,6 @@
     <t>doc2vec: use default parameter or find best practise</t>
   </si>
   <si>
-    <t>infersent: both vocab and trained?</t>
-  </si>
-  <si>
-    <t>infersent: provide smaller word2vec vocab?</t>
-  </si>
-  <si>
     <t>new times for embeddings</t>
   </si>
   <si>
@@ -339,6 +333,12 @@
   </si>
   <si>
     <t>BA: infersent, custom w2v for infersent</t>
+  </si>
+  <si>
+    <t>BA: SBERT (Hf)</t>
+  </si>
+  <si>
+    <t>BA: USE (google)</t>
   </si>
 </sst>
 </file>
@@ -896,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1427,7 +1427,7 @@
         <v>45199</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1435,7 +1435,7 @@
         <v>45200</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1443,18 +1443,30 @@
         <v>45201</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13">
+        <v>45202</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>100</v>
+      </c>
       <c r="D55" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="13">
+        <v>45203</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>99</v>
+      </c>
       <c r="D56" s="8" t="s">
         <v>86</v>
       </c>
@@ -1477,16 +1489,6 @@
     <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D60" s="8" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D61" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D62" s="8" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: re-inserted PCA OPTICS cluster into db
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB0AA9D-8240-0D4F-94BC-FCF6962F9343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E64438-FB8D-CF48-99AA-D009FC95DA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="560" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
   <si>
     <t>Task</t>
   </si>
@@ -339,6 +339,30 @@
   </si>
   <si>
     <t>BA: USE (google)</t>
+  </si>
+  <si>
+    <t>fix: tfidf on server</t>
+  </si>
+  <si>
+    <t>fix: connect to db on vscode</t>
+  </si>
+  <si>
+    <t>2971 docs inserted on server db, BA: topic modeling init</t>
+  </si>
+  <si>
+    <t>PCA &amp; cluster in DB</t>
+  </si>
+  <si>
+    <t>BA: PCA dim update</t>
+  </si>
+  <si>
+    <t>BERTopic</t>
+  </si>
+  <si>
+    <t>LDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -896,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1471,12 +1495,24 @@
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="13">
+        <v>45204</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>103</v>
+      </c>
       <c r="D57" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="13">
+        <v>45205</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>104</v>
+      </c>
       <c r="D58" s="8" t="s">
         <v>88</v>
       </c>
@@ -1487,8 +1523,36 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B60" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="D60" s="8" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D61" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D62" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D64" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D65" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D66" s="8" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: ae if tfidf emb > 2048 dims
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EDF107-C433-934F-AEE3-7E9E815EA6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0EA68B-492F-704C-9054-1293BDF1F3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
   <si>
     <t>Task</t>
   </si>
@@ -350,9 +350,6 @@
     <t>2971 docs inserted on server db, BA: topic modeling init</t>
   </si>
   <si>
-    <t>BA: PCA dim update</t>
-  </si>
-  <si>
     <t>BERTopic</t>
   </si>
   <si>
@@ -365,7 +362,7 @@
     <t>run times_per_emb on server</t>
   </si>
   <si>
-    <t>PCA &amp; cluster in DB, argmax PCA cluster</t>
+    <t>PCA &amp; cluster in DB, argmax PCA cluster, BA: PCA dim update, BA: bulk Elasticsearch</t>
   </si>
 </sst>
 </file>
@@ -530,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -603,6 +600,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1509,12 +1509,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>45205</v>
       </c>
-      <c r="B58" s="14" t="s">
-        <v>109</v>
+      <c r="B58" s="25" t="s">
+        <v>108</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>88</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B60" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>90</v>
@@ -1545,22 +1545,17 @@
     </row>
     <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D63" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D64" s="8" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D65" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D66" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Top2Vec works (BERTopic & LDA2Vec not)
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0EA68B-492F-704C-9054-1293BDF1F3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615968D9-C31F-D344-997C-024310218DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
   <si>
     <t>Task</t>
   </si>
@@ -363,6 +363,15 @@
   </si>
   <si>
     <t>PCA &amp; cluster in DB, argmax PCA cluster, BA: PCA dim update, BA: bulk Elasticsearch</t>
+  </si>
+  <si>
+    <t>Topic2Vec</t>
+  </si>
+  <si>
+    <t>LDA visualization from paper</t>
+  </si>
+  <si>
+    <t>LDA2Vec: does not work (import problem)</t>
   </si>
 </sst>
 </file>
@@ -527,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -600,9 +609,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -923,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1513,7 +1519,7 @@
       <c r="A58" s="13">
         <v>45205</v>
       </c>
-      <c r="B58" s="25" t="s">
+      <c r="B58" s="14" t="s">
         <v>108</v>
       </c>
       <c r="D58" s="8" t="s">
@@ -1556,6 +1562,21 @@
     <row r="66" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D66" s="8" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D67" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D68" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D69" s="8" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: more memory for universal sentence encoder
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AAEA0D-7544-3E4C-BB82-31E4FE7C7462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6F824E-6A37-4D4C-AAE4-C146AFCE27A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="0" yWindow="1240" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
   <si>
     <t>Task</t>
   </si>
@@ -344,9 +344,6 @@
     <t>fix: tfidf on server</t>
   </si>
   <si>
-    <t>fix: connect to db on vscode</t>
-  </si>
-  <si>
     <t>2971 docs inserted on server db, BA: topic modeling init</t>
   </si>
   <si>
@@ -374,10 +371,10 @@
     <t>Top2Vec code</t>
   </si>
   <si>
-    <t>FE: Topic2Vec</t>
-  </si>
-  <si>
     <t>new environment with python 12 to fix LDA and BERTopic</t>
+  </si>
+  <si>
+    <t>FE: Topic2Vec, fix: connect to db on vscode</t>
   </si>
 </sst>
 </file>
@@ -938,7 +935,7 @@
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1515,7 +1512,7 @@
         <v>45204</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>87</v>
@@ -1526,7 +1523,7 @@
         <v>45205</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>88</v>
@@ -1537,7 +1534,7 @@
         <v>45206</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>89</v>
@@ -1548,7 +1545,7 @@
         <v>45207</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>90</v>
@@ -1565,39 +1562,34 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D62" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
     <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D63" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D65" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D66" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D67" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D68" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D69" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: try less images to train pca
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6F824E-6A37-4D4C-AAE4-C146AFCE27A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60D31CF-32AE-DF43-B582-B0E8CDAA7777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1240" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
   <si>
     <t>Task</t>
   </si>
@@ -375,6 +375,9 @@
   </si>
   <si>
     <t>FE: Topic2Vec, fix: connect to db on vscode</t>
+  </si>
+  <si>
+    <t>tfidf, univ, pca/clusters on server</t>
   </si>
 </sst>
 </file>
@@ -932,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1592,6 +1595,11 @@
         <v>107</v>
       </c>
     </row>
+    <row r="70" spans="4:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D70" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:A5"/>

</xml_diff>

<commit_message>
fix: TFIDF preprocessing omitting punctions
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60D31CF-32AE-DF43-B582-B0E8CDAA7777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6068D125-78A4-704A-8C2F-0356E02B4555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1240" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="115">
   <si>
     <t>Task</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>tfidf, univ, pca/clusters on server</t>
+  </si>
+  <si>
+    <t>fix TfidfProcessor Preprocessing (punctations into ' ')</t>
   </si>
 </sst>
 </file>
@@ -937,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1565,7 +1568,19 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="13">
+        <v>45179</v>
+      </c>
+      <c r="B62" s="14"/>
+    </row>
+    <row r="63" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="13">
+        <v>45180</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>114</v>
+      </c>
       <c r="D63" s="8" t="s">
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
fix: try other node
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6068D125-78A4-704A-8C2F-0356E02B4555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2D78C1-B7B4-9A40-9165-DB9D6E8C7710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -380,7 +380,7 @@
     <t>tfidf, univ, pca/clusters on server</t>
   </si>
   <si>
-    <t>fix TfidfProcessor Preprocessing (punctations into ' ')</t>
+    <t>fix TfidfProcessor Preprocessing (punctations into ' '), fix clusters locally</t>
   </si>
 </sst>
 </file>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="B62" s="14"/>
     </row>
-    <row r="63" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>45180</v>
       </c>

</xml_diff>

<commit_message>
fix: tfidf + ae
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2D78C1-B7B4-9A40-9165-DB9D6E8C7710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D29704-3A58-D544-BF27-5FA3F68A0574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="-36760" yWindow="1180" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -377,10 +377,10 @@
     <t>FE: Topic2Vec, fix: connect to db on vscode</t>
   </si>
   <si>
-    <t>tfidf, univ, pca/clusters on server</t>
-  </si>
-  <si>
-    <t>fix TfidfProcessor Preprocessing (punctations into ' '), fix clusters locally</t>
+    <t>fix TfidfProcessor Preprocessing (punctations into ' '), fix clusters locally, universal sentenc on server</t>
+  </si>
+  <si>
+    <t>tfidf, pca/clusters on server</t>
   </si>
 </sst>
 </file>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1579,7 +1579,7 @@
         <v>45180</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>105</v>
@@ -1612,7 +1612,7 @@
     </row>
     <row r="70" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D70" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: list of docs as tfidf input
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D29704-3A58-D544-BF27-5FA3F68A0574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5F7EE6-DD3F-434A-9D6D-1FC8FB47CBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36760" yWindow="1180" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
   <si>
     <t>Task</t>
   </si>
@@ -381,6 +381,9 @@
   </si>
   <si>
     <t>tfidf, pca/clusters on server</t>
+  </si>
+  <si>
+    <t>topic modelling FE: search button to start search</t>
   </si>
 </sst>
 </file>
@@ -938,10 +941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1615,6 +1618,11 @@
         <v>114</v>
       </c>
     </row>
+    <row r="71" spans="4:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D71" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:A5"/>

</xml_diff>

<commit_message>
chore: plot for BA
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF986C1-0F4A-4F42-BBEF-90E0667BF61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681250AA-A76C-D84C-9F92-A247FCACD9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="120">
   <si>
     <t>Task</t>
   </si>
@@ -341,9 +341,6 @@
     <t>BA: USE (google)</t>
   </si>
   <si>
-    <t>fix: tfidf on server</t>
-  </si>
-  <si>
     <t>2971 docs inserted on server db, BA: topic modeling init</t>
   </si>
   <si>
@@ -390,6 +387,9 @@
   </si>
   <si>
     <t>tfidf on cluster</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>read BA</t>
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:B68"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1533,7 +1533,7 @@
         <v>45204</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>87</v>
@@ -1544,7 +1544,7 @@
         <v>45205</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>88</v>
@@ -1555,7 +1555,7 @@
         <v>45206</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>89</v>
@@ -1566,10 +1566,7 @@
         <v>45207</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1577,10 +1574,10 @@
         <v>45208</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1594,25 +1591,29 @@
         <v>45180</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
         <v>45181</v>
       </c>
-      <c r="B64" s="14"/>
+      <c r="B64" s="14" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="65" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
         <v>45182</v>
       </c>
-      <c r="B65" s="14"/>
+      <c r="B65" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="D65" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1620,10 +1621,10 @@
         <v>45183</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1634,7 +1635,7 @@
         <v>118</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1645,27 +1646,31 @@
         <v>119</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="13">
+        <v>45186</v>
+      </c>
+      <c r="B69" s="14"/>
       <c r="D69" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D70" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D71" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D72" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: parallelize insertion of embeddings
</commit_message>
<xml_diff>
--- a/organization/BA_tasks.xlsx
+++ b/organization/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681250AA-A76C-D84C-9F92-A247FCACD9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251AA140-857D-2347-9214-70E359894081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="-36920" yWindow="-380" windowWidth="34560" windowHeight="20520" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="131">
   <si>
     <t>Task</t>
   </si>
@@ -396,6 +396,39 @@
   </si>
   <si>
     <t>PCA &amp; OPTICS &amp; argmax cluster in DB on server</t>
+  </si>
+  <si>
+    <t>BA: shorter Listing &amp; Figure captions</t>
+  </si>
+  <si>
+    <t>PCA: reconstruction error only L knee</t>
+  </si>
+  <si>
+    <t>PCA: #comp &gt; 13, try on server with more data and higher maximum number</t>
+  </si>
+  <si>
+    <t>AE: let server try more possible architectures</t>
+  </si>
+  <si>
+    <t>Parallelize DB</t>
+  </si>
+  <si>
+    <t>run BE &amp; FE on server, make SSH Tunnel and use URL locally for UI and db from server</t>
+  </si>
+  <si>
+    <t>selection of documents: use random choice per directory path</t>
+  </si>
+  <si>
+    <t>BA: min. 50, max. 100 pages</t>
+  </si>
+  <si>
+    <t>BA: omit lists at the end</t>
+  </si>
+  <si>
+    <t>BA: SE template is ok</t>
+  </si>
+  <si>
+    <t>TFIDF: custom preprocessing \W for all white spaces</t>
   </si>
 </sst>
 </file>
@@ -560,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -632,6 +665,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -953,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,7 +1415,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="18">
+      <c r="A42" s="25">
         <v>45189</v>
       </c>
       <c r="B42" s="14" t="s">
@@ -1653,12 +1689,20 @@
       <c r="A69" s="13">
         <v>45186</v>
       </c>
-      <c r="B69" s="14"/>
+      <c r="B69" s="14" t="s">
+        <v>120</v>
+      </c>
       <c r="D69" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="18">
+        <v>45187</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>130</v>
+      </c>
       <c r="D70" s="8" t="s">
         <v>113</v>
       </c>
@@ -1671,6 +1715,51 @@
     <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D72" s="8" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D73" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="D74" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D75" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D77" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="D78" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D79" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D80" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D81" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D82" s="8" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>